<commit_message>
Revert capacity charts to show kilowatts on the y-axis. Changes to facilities charts are incidental. Corresponding code changes coming in the next commit.
</commit_message>
<xml_diff>
--- a/output_data/charts/capacity-15-CountyRegion-M010000US001.xlsx
+++ b/output_data/charts/capacity-15-CountyRegion-M010000US001.xlsx
@@ -42,7 +42,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -295,7 +295,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>400000</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -486,7 +486,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4000000</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -498,28 +498,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>100000</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>250000</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>600000</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>78280</c:v>
+                  <c:v>78.28</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>132760</c:v>
+                  <c:v>132.76</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>438670</c:v>
+                  <c:v>438.67</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1558120</c:v>
+                  <c:v>1558.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -683,7 +683,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>248000</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -692,7 +692,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15036000</c:v>
+                  <c:v>15036</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -707,7 +707,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4804000</c:v>
+                  <c:v>4804</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0</c:v>
@@ -844,64 +844,64 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1650</c:v>
+                  <c:v>1.65</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13860</c:v>
+                  <c:v>13.86</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25050</c:v>
+                  <c:v>25.05</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>69300</c:v>
+                  <c:v>69.3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>77400</c:v>
+                  <c:v>77.40000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>445490</c:v>
+                  <c:v>445.49</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1305165</c:v>
+                  <c:v>1305.165</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6853460</c:v>
+                  <c:v>6853.46</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1690355</c:v>
+                  <c:v>1690.355</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2244240</c:v>
+                  <c:v>2244.24</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1400320</c:v>
+                  <c:v>1400.32</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1373165</c:v>
+                  <c:v>1373.165</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4905780</c:v>
+                  <c:v>4905.78</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2522110</c:v>
+                  <c:v>2522.11</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6608960</c:v>
+                  <c:v>6608.96</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4931880</c:v>
+                  <c:v>4931.88</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8520562</c:v>
+                  <c:v>8520.562</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10393910</c:v>
+                  <c:v>10393.91</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23772402</c:v>
+                  <c:v>23772.402</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>13681038</c:v>
+                  <c:v>13681.038</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1071,7 +1071,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3500000</c:v>
+                  <c:v>3500</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -1211,10 +1211,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>10000</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18000</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1223,10 +1223,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1000</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8000</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1235,22 +1235,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1800</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>47800</c:v>
+                  <c:v>47.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>161800</c:v>
+                  <c:v>161.8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2400</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1500</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30000</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -1265,7 +1265,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4500000</c:v>
+                  <c:v>4500</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -1342,14 +1342,14 @@
                   <a:rPr lang="en-US" sz="900" baseline="0">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Watts</a:t>
+                  <a:t>Kilowatts (kW)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="[&gt;=1000]#,##0,&quot;K&quot;" sourceLinked="0"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="low"/>
         <c:txPr>
           <a:bodyPr/>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <v>10000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1795,7 +1795,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="2">
-        <v>18000</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1864,7 +1864,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="2">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1881,13 +1881,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="2">
-        <v>1650</v>
+        <v>1.65</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="2">
-        <v>8000</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>13860</v>
+        <v>13.86</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2">
-        <v>25050</v>
+        <v>25.05</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
@@ -1950,13 +1950,13 @@
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <v>69300</v>
+        <v>69.3</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
       </c>
       <c r="G10" s="2">
-        <v>1800</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1973,13 +1973,13 @@
         <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>77400</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
       </c>
       <c r="G11" s="2">
-        <v>47800</v>
+        <v>47.8</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1996,13 +1996,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="2">
-        <v>445490</v>
+        <v>445.49</v>
       </c>
       <c r="F12" s="2">
         <v>0</v>
       </c>
       <c r="G12" s="2">
-        <v>161800</v>
+        <v>161.8</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2019,13 +2019,13 @@
         <v>0</v>
       </c>
       <c r="E13" s="2">
-        <v>1305165</v>
+        <v>1305.165</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
       </c>
       <c r="G13" s="2">
-        <v>2400</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2042,13 +2042,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="2">
-        <v>6853460</v>
+        <v>6853.46</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
       </c>
       <c r="G14" s="2">
-        <v>1500</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2056,22 +2056,22 @@
         <v>2013</v>
       </c>
       <c r="B15" s="2">
-        <v>400000</v>
+        <v>400</v>
       </c>
       <c r="C15" s="2">
-        <v>4000000</v>
+        <v>4000</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
       </c>
       <c r="E15" s="2">
-        <v>1690355</v>
+        <v>1690.355</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="2">
-        <v>30000</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="2">
-        <v>2244240</v>
+        <v>2244.24</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
@@ -2108,10 +2108,10 @@
         <v>0</v>
       </c>
       <c r="D17" s="2">
-        <v>248000</v>
+        <v>248</v>
       </c>
       <c r="E17" s="2">
-        <v>1400320</v>
+        <v>1400.32</v>
       </c>
       <c r="F17" s="2">
         <v>0</v>
@@ -2134,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="2">
-        <v>1373165</v>
+        <v>1373.165</v>
       </c>
       <c r="F18" s="2">
         <v>0</v>
@@ -2151,16 +2151,16 @@
         <v>0</v>
       </c>
       <c r="C19" s="2">
-        <v>100000</v>
+        <v>100</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
       </c>
       <c r="E19" s="2">
-        <v>4905780</v>
+        <v>4905.78</v>
       </c>
       <c r="F19" s="2">
-        <v>3500000</v>
+        <v>3500</v>
       </c>
       <c r="G19" s="2">
         <v>0</v>
@@ -2177,16 +2177,16 @@
         <v>0</v>
       </c>
       <c r="D20" s="2">
-        <v>15036000</v>
+        <v>15036</v>
       </c>
       <c r="E20" s="2">
-        <v>2522110</v>
+        <v>2522.11</v>
       </c>
       <c r="F20" s="2">
         <v>0</v>
       </c>
       <c r="G20" s="2">
-        <v>4500000</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2197,13 +2197,13 @@
         <v>0</v>
       </c>
       <c r="C21" s="2">
-        <v>250000</v>
+        <v>250</v>
       </c>
       <c r="D21" s="2">
         <v>0</v>
       </c>
       <c r="E21" s="2">
-        <v>6608960</v>
+        <v>6608.96</v>
       </c>
       <c r="F21" s="2">
         <v>0</v>
@@ -2220,13 +2220,13 @@
         <v>0</v>
       </c>
       <c r="C22" s="2">
-        <v>600000</v>
+        <v>600</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
       </c>
       <c r="E22" s="2">
-        <v>4931880</v>
+        <v>4931.88</v>
       </c>
       <c r="F22" s="2">
         <v>0</v>
@@ -2243,13 +2243,13 @@
         <v>0</v>
       </c>
       <c r="C23" s="2">
-        <v>78280</v>
+        <v>78.28</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
       </c>
       <c r="E23" s="2">
-        <v>8520562</v>
+        <v>8520.562</v>
       </c>
       <c r="F23" s="2">
         <v>0</v>
@@ -2266,13 +2266,13 @@
         <v>0</v>
       </c>
       <c r="C24" s="2">
-        <v>132760</v>
+        <v>132.76</v>
       </c>
       <c r="D24" s="2">
         <v>0</v>
       </c>
       <c r="E24" s="2">
-        <v>10393910</v>
+        <v>10393.91</v>
       </c>
       <c r="F24" s="2">
         <v>0</v>
@@ -2289,13 +2289,13 @@
         <v>0</v>
       </c>
       <c r="C25" s="2">
-        <v>438670</v>
+        <v>438.67</v>
       </c>
       <c r="D25" s="2">
-        <v>4804000</v>
+        <v>4804</v>
       </c>
       <c r="E25" s="2">
-        <v>23772402</v>
+        <v>23772.402</v>
       </c>
       <c r="F25" s="2">
         <v>0</v>
@@ -2312,13 +2312,13 @@
         <v>0</v>
       </c>
       <c r="C26" s="2">
-        <v>1558120</v>
+        <v>1558.12</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
       </c>
       <c r="E26" s="2">
-        <v>13681038</v>
+        <v>13681.038</v>
       </c>
       <c r="F26" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Incorporate updated data from upstream processes through 2024
</commit_message>
<xml_diff>
--- a/output_data/charts/capacity-15-CountyRegion-M010000US001.xlsx
+++ b/output_data/charts/capacity-15-CountyRegion-M010000US001.xlsx
@@ -519,7 +519,7 @@
                   <c:v>438.67</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1558.12</c:v>
+                  <c:v>1642.24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -874,7 +874,7 @@
                   <c:v>2244.24</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1400.32</c:v>
+                  <c:v>1399.48</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1373.165</c:v>
@@ -892,16 +892,16 @@
                   <c:v>4931.88</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8520.562</c:v>
+                  <c:v>8517.262000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10393.91</c:v>
+                  <c:v>10409.82</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23772.402</c:v>
+                  <c:v>23790.902</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>13681.038</c:v>
+                  <c:v>20800.418</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2111,7 +2111,7 @@
         <v>248</v>
       </c>
       <c r="E17" s="2">
-        <v>1400.32</v>
+        <v>1399.48</v>
       </c>
       <c r="F17" s="2">
         <v>0</v>
@@ -2249,7 +2249,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="2">
-        <v>8520.562</v>
+        <v>8517.262000000001</v>
       </c>
       <c r="F23" s="2">
         <v>0</v>
@@ -2272,7 +2272,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="2">
-        <v>10393.91</v>
+        <v>10409.82</v>
       </c>
       <c r="F24" s="2">
         <v>0</v>
@@ -2295,7 +2295,7 @@
         <v>4804</v>
       </c>
       <c r="E25" s="2">
-        <v>23772.402</v>
+        <v>23790.902</v>
       </c>
       <c r="F25" s="2">
         <v>0</v>
@@ -2312,13 +2312,13 @@
         <v>0</v>
       </c>
       <c r="C26" s="2">
-        <v>1558.12</v>
+        <v>1642.24</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
       </c>
       <c r="E26" s="2">
-        <v>13681.038</v>
+        <v>20800.418</v>
       </c>
       <c r="F26" s="2">
         <v>0</v>

</xml_diff>